<commit_message>
Added Tuning notebooks for CatBoost and Extra Trees Output
</commit_message>
<xml_diff>
--- a/Kip/ML/PyCaret Model Guide.xlsx
+++ b/Kip/ML/PyCaret Model Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kip Madden\Desktop\dataScience\Project3\Kip\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB9B8B8-6CC0-4DE8-B885-6A84DF3486C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B267E7A-0729-4925-B2C1-E0E33D8AC023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{EAB88605-644A-45DC-A1E5-601E8C31A39C}"/>
+    <workbookView xWindow="48240" yWindow="171" windowWidth="17409" windowHeight="17563" activeTab="1" xr2:uid="{EAB88605-644A-45DC-A1E5-601E8C31A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Modeling" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="89">
   <si>
     <t>Classification</t>
   </si>
@@ -283,25 +283,25 @@
     <t>NOT for multiclass</t>
   </si>
   <si>
-    <t>Interpret</t>
-  </si>
-  <si>
-    <t>Correlation</t>
-  </si>
-  <si>
-    <t>correlation'</t>
-  </si>
-  <si>
     <t>interpret_model()</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
     <t>Reason</t>
   </si>
   <si>
     <t>reason'</t>
+  </si>
+  <si>
+    <t>plot='summary'</t>
+  </si>
+  <si>
+    <t>plot='correlation'</t>
+  </si>
+  <si>
+    <t>feature='  '</t>
+  </si>
+  <si>
+    <t>Medium Speed        Must have Node.js installed</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -524,11 +524,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -584,22 +621,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1109,7 +1159,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1124,30 +1174,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="D1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1156,10 +1206,10 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="28.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -1168,8 +1218,8 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>80</v>
+      <c r="D4" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>80</v>
@@ -1268,8 +1318,8 @@
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>80</v>
+      <c r="D9" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>80</v>
@@ -1345,8 +1395,8 @@
       <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>80</v>
+      <c r="D13" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>80</v>
@@ -1365,8 +1415,8 @@
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>80</v>
+      <c r="D14" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>80</v>
@@ -1394,6 +1444,9 @@
       <c r="F15" s="13" t="s">
         <v>76</v>
       </c>
+      <c r="G15" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="28.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
@@ -1428,6 +1481,9 @@
       <c r="F17" s="14" t="s">
         <v>80</v>
       </c>
+      <c r="G17" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="28.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
@@ -1445,24 +1501,25 @@
       <c r="F18" s="14" t="s">
         <v>80</v>
       </c>
+      <c r="G18" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="26" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>80</v>
+      <c r="B20" s="27"/>
+      <c r="D20" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>80</v>
@@ -1473,13 +1530,13 @@
     </row>
     <row r="21" spans="1:9" ht="37.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>80</v>
@@ -1490,15 +1547,15 @@
     </row>
     <row r="22" spans="1:9" ht="33.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="28" t="s">
         <v>80</v>
       </c>
       <c r="F22" s="13" t="s">
@@ -1532,12 +1589,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1565,30 +1622,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="D1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1597,10 +1654,10 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="28.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -1845,12 +1902,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G3"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Excel PyCaret Model Guide & Added EPOCH1Best.ipynb
</commit_message>
<xml_diff>
--- a/Kip/ML/PyCaret Model Guide.xlsx
+++ b/Kip/ML/PyCaret Model Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kip Madden\Desktop\dataScience\Project3\Kip\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E8FD40-3E4F-440F-9836-DBFDECCF2806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82784DBF-AEFC-4908-AB93-699DD76CA1B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{EAB88605-644A-45DC-A1E5-601E8C31A39C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="97">
   <si>
     <t>Classification</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>plot_model()</t>
+  </si>
+  <si>
+    <t>`za</t>
   </si>
 </sst>
 </file>
@@ -659,6 +662,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -671,43 +707,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1217,7 +1220,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1232,30 +1235,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="38"/>
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="36" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
@@ -1264,10 +1267,10 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
@@ -1276,16 +1279,16 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="36" t="s">
+      <c r="D4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1296,16 +1299,16 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="35" t="s">
+      <c r="D5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1316,16 +1319,18 @@
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="21"/>
+      <c r="D6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
@@ -1334,7 +1339,7 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="29" t="s">
         <v>76</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1352,16 +1357,16 @@
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="36" t="s">
+      <c r="D8" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1372,16 +1377,16 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="36" t="s">
+      <c r="D9" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1392,16 +1397,16 @@
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="36" t="s">
+      <c r="D10" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1412,16 +1417,16 @@
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="36" t="s">
+      <c r="D11" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1432,16 +1437,16 @@
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="36" t="s">
+      <c r="D12" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1452,13 +1457,13 @@
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="39" t="s">
+      <c r="D13" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="29" t="s">
         <v>81</v>
       </c>
       <c r="G13" s="21"/>
@@ -1470,16 +1475,16 @@
       <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="30" t="s">
+      <c r="D14" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1490,16 +1495,16 @@
       <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="38" t="s">
+      <c r="D15" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1510,16 +1515,16 @@
       <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="35" t="s">
+      <c r="D16" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1530,16 +1535,16 @@
       <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="30" t="s">
+      <c r="D17" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="38" t="s">
+      <c r="F17" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1550,13 +1555,13 @@
       <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="36" t="s">
+      <c r="D18" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G18" s="21"/>
@@ -1568,16 +1573,16 @@
       <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="36" t="s">
+      <c r="D19" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1588,16 +1593,16 @@
       <c r="B20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="36" t="s">
+      <c r="D20" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1617,10 +1622,10 @@
       <c r="D22" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="35" t="s">
+      <c r="E22" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="29" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1634,10 +1639,10 @@
       <c r="D23" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="35" t="s">
+      <c r="E23" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="29" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1651,32 +1656,32 @@
       <c r="D24" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="35" t="s">
+      <c r="E24" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="29" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="26" spans="1:9" ht="29.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="D26" s="29" t="s">
+      <c r="B26" s="35"/>
+      <c r="D26" s="23" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="H26" s="26" t="s">
         <v>37</v>
       </c>
       <c r="I26" s="13" t="s">
@@ -1684,22 +1689,22 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G27" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="H27" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="28" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1738,30 +1743,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="38"/>
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1770,10 +1775,10 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" ht="28.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -1993,10 +1998,10 @@
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="1:9" ht="29.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="35"/>
       <c r="D22" s="14" t="s">
         <v>36</v>
       </c>

</xml_diff>